<commit_message>
updated codegen to use Onix 3.0 rev 07 + Codelist issue 49
</commit_message>
<xml_diff>
--- a/jonix-codegen/src/main/resources/xsd-revision-history.xlsx
+++ b/jonix-codegen/src/main/resources/xsd-revision-history.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Jonix\jonix\jonix-codegen\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EAD0A9-F996-431B-AE5F-C89AF95084AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{29A5436D-5A35-4569-9299-10232424BEFA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12223"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Progress" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Revision</t>
   </si>
@@ -340,13 +339,22 @@
   </si>
   <si>
     <t>Revision-Date</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_49_v1-7-2.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_49.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_49.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +364,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -387,12 +403,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +428,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -476,7 +493,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94618CB4-E42A-4959-9139-D8738230BEF3}" type="CELLRANGE">
+                    <a:fld id="{9538687D-5168-4FE2-83D0-85B90762D1C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -497,9 +514,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -509,7 +523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18AABD46-D0F7-4F29-9F19-C6556B8260F7}" type="CELLRANGE">
+                    <a:fld id="{190B3FC9-E849-4CA8-A43B-DF972C51C97B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -530,9 +544,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -542,7 +553,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{393F908E-63EA-48B4-9FD7-9DD6B6FDF750}" type="CELLRANGE">
+                    <a:fld id="{BE52D925-9F9D-427F-B62B-F072C05883EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -563,9 +574,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -575,7 +583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC828142-B7A3-4CDF-9B96-CB1F94495991}" type="CELLRANGE">
+                    <a:fld id="{41A5D316-0A59-4747-ADE0-EC1D51A082BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -596,9 +604,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -608,7 +613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03B01269-5E55-485F-9E1A-EB6F4265F503}" type="CELLRANGE">
+                    <a:fld id="{0959F088-EF67-494C-998C-9F57C6DC8A44}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -629,9 +634,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -641,7 +643,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44148BE8-5272-4528-BB54-2BF7D5210491}" type="CELLRANGE">
+                    <a:fld id="{890334E1-21CB-4E6D-9C84-7142AF7FB1DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -662,9 +664,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -674,7 +673,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22F867AD-8041-42CA-B987-039988BFC1C0}" type="CELLRANGE">
+                    <a:fld id="{74491469-0BF1-421A-9748-8AC8795B713A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -695,9 +694,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -707,7 +703,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3F8BC53-155B-4FD5-88F8-3D2840C954DB}" type="CELLRANGE">
+                    <a:fld id="{2269D38D-E085-4B69-947B-2B5C26ECC6B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -728,9 +724,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -740,7 +733,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A539D43A-177A-4C62-BC78-803714216115}" type="CELLRANGE">
+                    <a:fld id="{9D87ED03-DF74-4BE7-89EE-AA7970A24159}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -761,9 +754,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -773,7 +763,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{508B0EB9-9DBF-4C77-9A43-D1130B525ECA}" type="CELLRANGE">
+                    <a:fld id="{0D636556-B298-41D2-9888-FFAD4E5CD8D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -794,9 +784,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -806,7 +793,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9D5FD99-BDA2-4A2F-A714-5E847D287A07}" type="CELLRANGE">
+                    <a:fld id="{EFA0160C-CDD1-42A6-A8E6-4F746C72BB6F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -827,9 +814,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -839,7 +823,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{77D046AB-1623-4872-BD06-B06E03D63655}" type="CELLRANGE">
+                    <a:fld id="{06BB29E1-5C7D-4B70-A609-BE525B5ECE15}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -860,9 +844,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000D-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -872,7 +853,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83FF7313-904F-4E1B-92ED-67B4D6387F66}" type="CELLRANGE">
+                    <a:fld id="{18A902B6-BB91-4FD5-B709-5393E650B675}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -893,9 +874,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000E-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -905,7 +883,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7B02B58F-E45B-498F-9DC3-83F6E208A2BF}" type="CELLRANGE">
+                    <a:fld id="{918CD4E5-FC8A-4F6C-949B-7E78149136A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -926,9 +904,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000F-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -938,7 +913,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22E0AA16-FCDC-4C1E-99CB-F0871423BD6E}" type="CELLRANGE">
+                    <a:fld id="{9DC051D2-32A5-4507-91B7-8382FAD12220}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -959,9 +934,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000010-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -971,7 +943,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DB41B66-7E40-4682-AB26-6B24DA902159}" type="CELLRANGE">
+                    <a:fld id="{4687C1F2-E486-4ECC-9CD6-60FBA170C164}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -992,9 +964,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000011-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1004,7 +973,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA39A3C0-B73E-4F96-B8F9-F393AC4A6A99}" type="CELLRANGE">
+                    <a:fld id="{6AF0FE44-D572-4F76-A1E5-949E322167ED}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1025,9 +994,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000012-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1037,7 +1003,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CAB96088-EF44-4C0A-AB0B-8750A2C8558F}" type="CELLRANGE">
+                    <a:fld id="{CAB0B527-C39E-413C-BF8A-CCDAFF3F4998}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1058,9 +1024,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000013-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1070,7 +1033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F116159-13B8-4B08-B564-34C4737762D4}" type="CELLRANGE">
+                    <a:fld id="{FC2FB84F-FF96-48BF-9CFF-40EB5CE932A4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1091,9 +1054,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000014-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1103,7 +1063,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{629087D3-CD67-4D0D-8024-72819182306C}" type="CELLRANGE">
+                    <a:fld id="{781870A7-508E-430E-A5B8-43EDF3C1989D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1124,9 +1084,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000015-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1136,7 +1093,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B93FE1CB-A2D0-4455-8A6A-DD0D0E1C29DB}" type="CELLRANGE">
+                    <a:fld id="{65520891-405F-4A24-B982-41681C1874F9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1157,9 +1114,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000016-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1169,7 +1123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3B921F9-0B58-4D89-9199-0A65253DF66A}" type="CELLRANGE">
+                    <a:fld id="{C7826E9D-B5EE-46A2-8C10-E6E84AB5702E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1190,9 +1144,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000017-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1202,7 +1153,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60EC99E7-7187-4CCD-8139-767F3E04AB34}" type="CELLRANGE">
+                    <a:fld id="{B288BC7E-98BD-4677-8AE9-89759D8172B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1223,9 +1174,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000018-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1235,7 +1183,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0036135B-52EA-4908-98C9-547A6FE4D720}" type="CELLRANGE">
+                    <a:fld id="{8C85AD00-17ED-4EDD-AC99-DE4BEF8D007F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1256,9 +1204,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000019-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1268,7 +1213,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C8212E6-ACC2-415B-8D24-E9988F52ACF3}" type="CELLRANGE">
+                    <a:fld id="{8C482FBB-F854-4EDB-9A1B-0F358E0B6872}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1289,9 +1234,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000001A-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1301,7 +1243,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A941DDFC-B0E5-4036-817F-05F012D9BD62}" type="CELLRANGE">
+                    <a:fld id="{A93D59F8-900F-4E24-82B4-0E677917A5FA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1322,9 +1264,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000001B-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1334,7 +1273,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E17D86C-7170-49F5-8974-74878A5D4887}" type="CELLRANGE">
+                    <a:fld id="{A5A2ACB4-4C92-45EE-833D-D28192A2C1B1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1355,9 +1294,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000001C-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1367,7 +1303,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89BB5DF8-0D5E-46AD-9275-BE3220C24DFE}" type="CELLRANGE">
+                    <a:fld id="{2F924EB0-14F3-41D7-AAAB-83BBE4E6A71D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1388,9 +1324,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000001D-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1400,7 +1333,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD71B0F1-0D5C-4BE9-83BA-94796EEF6FCB}" type="CELLRANGE">
+                    <a:fld id="{BBF4A9F6-8BED-4FD2-988D-51C1D20B376D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1421,9 +1354,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000001E-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1433,7 +1363,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C88CD17F-AD78-4BE1-9151-1C14F1847718}" type="CELLRANGE">
+                    <a:fld id="{6B1BCD0B-3CFE-4940-82D4-A260DDC002E8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1454,9 +1384,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000001F-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1466,7 +1393,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95C9B9AD-FAB2-4ECD-8D33-9D627FEB6F88}" type="CELLRANGE">
+                    <a:fld id="{87E61112-C826-400E-AC05-040C9005D93C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1487,9 +1414,6 @@
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000020-A9B9-4699-85A7-BBCAE1008CF9}"/>
-                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1499,7 +1423,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFB94856-1535-4743-B62B-6929B52B8867}" type="CELLRANGE">
+                    <a:fld id="{B5822CF3-9D55-4747-9033-55EC908E3403}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1519,9 +1443,6 @@
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000021-A9B9-4699-85A7-BBCAE1008CF9}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1561,7 +1482,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
@@ -1691,7 +1612,7 @@
             <c:numRef>
               <c:f>Data!$C$2:$C$33</c:f>
               <c:numCache>
-                <c:formatCode>dd-mm-yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>40694</c:v>
@@ -1793,7 +1714,10 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A9B9-4699-85A7-BBCAE1008CF9}"/>
+            </c:ext>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
                 <c15:f>Data!$B$2:$B$33</c15:f>
@@ -1898,9 +1822,6 @@
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A9B9-4699-85A7-BBCAE1008CF9}"/>
-            </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
@@ -2050,7 +1971,7 @@
             <c:numRef>
               <c:f>Data!$D$2:$D$33</c:f>
               <c:numCache>
-                <c:formatCode>dd-mm-yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>40721</c:v>
@@ -2152,7 +2073,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A9B9-4699-85A7-BBCAE1008CF9}"/>
             </c:ext>
@@ -2166,11 +2087,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="299818248"/>
-        <c:axId val="299814640"/>
+        <c:axId val="445961568"/>
+        <c:axId val="445961960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="299818248"/>
+        <c:axId val="445961568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2227,12 +2148,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299814640"/>
+        <c:crossAx val="445961960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="299814640"/>
+        <c:axId val="445961960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2252,7 +2173,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="dd-mm-yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2289,7 +2210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299818248"/>
+        <c:crossAx val="445961568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2334,14 +2255,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2928,7 +2849,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{79C71E96-763B-4E89-A128-AF457DC546B3}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
@@ -2948,7 +2869,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B75B44A-C79E-43F4-8C15-9CD5F5169534}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1B75B44A-C79E-43F4-8C15-9CD5F5169534}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3267,8 +3188,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3693C42-6E6D-4AC5-AC41-2E0B36BBD4A5}">
-  <dimension ref="A1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -3277,19 +3198,20 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="109.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="88.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="111.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.53515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="100.53515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="81.07421875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.15234375" style="5"/>
+    <col min="9" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3312,7 +3234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>14</v>
       </c>
@@ -3334,12 +3256,12 @@
       <c r="G2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="1" t="str">
+      <c r="H2" s="5" t="str">
         <f>"curl -O "&amp;G2</f>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_14.html</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>15</v>
       </c>
@@ -3361,12 +3283,12 @@
       <c r="G3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H33" si="0">"curl -O "&amp;G3</f>
+      <c r="H3" s="5" t="str">
+        <f t="shared" ref="H3:H34" si="0">"curl -O "&amp;G3</f>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_15.html</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>16</v>
       </c>
@@ -3388,12 +3310,12 @@
       <c r="G4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="1" t="str">
+      <c r="H4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_16.html</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>17</v>
       </c>
@@ -3415,12 +3337,12 @@
       <c r="G5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="1" t="str">
+      <c r="H5" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_17.html</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>18</v>
       </c>
@@ -3442,12 +3364,12 @@
       <c r="G6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="1" t="str">
+      <c r="H6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_18.html</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>19</v>
       </c>
@@ -3469,12 +3391,12 @@
       <c r="G7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="1" t="str">
+      <c r="H7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_19.html</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>20</v>
       </c>
@@ -3496,12 +3418,12 @@
       <c r="G8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="1" t="str">
+      <c r="H8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_20.html</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>21</v>
       </c>
@@ -3523,12 +3445,12 @@
       <c r="G9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="1" t="str">
+      <c r="H9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_21.html</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>22</v>
       </c>
@@ -3550,12 +3472,12 @@
       <c r="G10" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H10" s="1" t="str">
+      <c r="H10" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_22.html</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>23</v>
       </c>
@@ -3577,12 +3499,12 @@
       <c r="G11" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H11" s="1" t="str">
+      <c r="H11" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_23.html</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>24</v>
       </c>
@@ -3604,12 +3526,12 @@
       <c r="G12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H12" s="1" t="str">
+      <c r="H12" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_24.html</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>25</v>
       </c>
@@ -3631,12 +3553,12 @@
       <c r="G13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="1" t="str">
+      <c r="H13" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_25.html</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>26</v>
       </c>
@@ -3658,12 +3580,12 @@
       <c r="G14" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="1" t="str">
+      <c r="H14" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_26.html</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>27</v>
       </c>
@@ -3685,12 +3607,12 @@
       <c r="G15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="1" t="str">
+      <c r="H15" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_27.html</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>28</v>
       </c>
@@ -3712,12 +3634,12 @@
       <c r="G16" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H16" s="1" t="str">
+      <c r="H16" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_28.html</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>29</v>
       </c>
@@ -3739,12 +3661,12 @@
       <c r="G17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H17" s="1" t="str">
+      <c r="H17" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_29.html</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>30</v>
       </c>
@@ -3766,12 +3688,12 @@
       <c r="G18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="1" t="str">
+      <c r="H18" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_30.html</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>31</v>
       </c>
@@ -3793,12 +3715,12 @@
       <c r="G19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="1" t="str">
+      <c r="H19" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_31.html</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>32</v>
       </c>
@@ -3820,12 +3742,12 @@
       <c r="G20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H20" s="1" t="str">
+      <c r="H20" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_32.html</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>33</v>
       </c>
@@ -3847,12 +3769,12 @@
       <c r="G21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H21" s="1" t="str">
+      <c r="H21" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_33.html</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>34</v>
       </c>
@@ -3874,12 +3796,12 @@
       <c r="G22" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H22" s="1" t="str">
+      <c r="H22" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_34.html</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>35</v>
       </c>
@@ -3901,12 +3823,12 @@
       <c r="G23" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H23" s="1" t="str">
+      <c r="H23" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_35.html</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>36</v>
       </c>
@@ -3928,12 +3850,12 @@
       <c r="G24" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H24" s="1" t="str">
+      <c r="H24" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_36.html</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>37</v>
       </c>
@@ -3955,12 +3877,12 @@
       <c r="G25" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H25" s="1" t="str">
+      <c r="H25" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_37.html</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>38</v>
       </c>
@@ -3982,12 +3904,12 @@
       <c r="G26" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H26" s="1" t="str">
+      <c r="H26" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_38.html</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>39</v>
       </c>
@@ -4009,12 +3931,12 @@
       <c r="G27" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H27" s="1" t="str">
+      <c r="H27" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_39.html</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>40</v>
       </c>
@@ -4036,12 +3958,12 @@
       <c r="G28" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H28" s="1" t="str">
+      <c r="H28" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_40.html</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>41</v>
       </c>
@@ -4063,12 +3985,12 @@
       <c r="G29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H29" s="1" t="str">
+      <c r="H29" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_41.html</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>42</v>
       </c>
@@ -4090,12 +4012,12 @@
       <c r="G30" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H30" s="1" t="str">
+      <c r="H30" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_42.html</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>43</v>
       </c>
@@ -4117,12 +4039,12 @@
       <c r="G31" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H31" s="1" t="str">
+      <c r="H31" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_43.html</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>44</v>
       </c>
@@ -4144,12 +4066,12 @@
       <c r="G32" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H32" s="1" t="str">
+      <c r="H32" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_44.html</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>45</v>
       </c>
@@ -4171,9 +4093,36 @@
       <c r="G33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H33" s="1" t="str">
+      <c r="H33" s="5" t="str">
         <f t="shared" si="0"/>
         <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_45.html</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A34" s="1">
+        <v>49</v>
+      </c>
+      <c r="B34" s="1">
+        <v>7</v>
+      </c>
+      <c r="C34" s="3">
+        <v>43769</v>
+      </c>
+      <c r="D34" s="3">
+        <v>43907</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_49.html</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extracted xsd and other meta files for releases 50..58
</commit_message>
<xml_diff>
--- a/jonix-codegen/src/main/resources/xsd-revision-history.xlsx
+++ b/jonix-codegen/src/main/resources/xsd-revision-history.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Jonix\jonix\jonix-codegen\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV-ZACH\Jonix\jonix\jonix-codegen\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12223"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Progress" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Progress" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
   <si>
     <t>Revision</t>
   </si>
@@ -348,13 +349,85 @@
   </si>
   <si>
     <t>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_49.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *                   Revision 7                   *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *              Revised: 2020-05-18               *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *                   Revision 8                   *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *              Revised: 2021-04-29               *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *            Release date: 2020-07-09            *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *            Release date: 2020-10-20            *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *            Release date: 2021-01-25            *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *            Release date: 2021-06-29            *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *            Release date: 2021-10-28            *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *            Release date: 2022-01-21            *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *            Release date: 2022-04-12            *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *            Release date: 2022-07-18            *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        *            Release date: 2021-08-08            *</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_50_v1-7-3.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_56_v1-8-3.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_51_v1-7-4.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_57_v1-8-4.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_52_v1-7-5.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_53_v1-8-0.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_54_v1-8-1.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_55_v1-8-2.zip</t>
+  </si>
+  <si>
+    <t>https://www.editeur.org/files/ONIX%203/ONIX_for_Books_Release3-0_html_Best_Practice+codes_Issue_58_v1-8-5.zip</t>
+  </si>
+  <si>
+    <t>CURL Cmd</t>
+  </si>
+  <si>
+    <t>Label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +445,14 @@
       <i/>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -403,13 +484,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +513,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -488,17 +573,18 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9538687D-5168-4FE2-83D0-85B90762D1C6}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{6E353242-40AA-411A-BFF8-3E58BC457FA3}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -510,25 +596,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{190B3FC9-E849-4CA8-A43B-DF972C51C97B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{F9349DAD-0BBA-4330-90F6-6A72BDEA64D4}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -540,25 +631,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE52D925-9F9D-427F-B62B-F072C05883EE}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{AA2E5D46-445E-4042-83F1-BA5C7EE66615}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -570,25 +666,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{41A5D316-0A59-4747-ADE0-EC1D51A082BA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{6723A872-8F38-43E9-A12B-26D669A4C720}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -600,25 +701,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0959F088-EF67-494C-998C-9F57C6DC8A44}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{6080E2DC-B66F-4B65-A689-464AB73A9590}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -630,25 +736,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{890334E1-21CB-4E6D-9C84-7142AF7FB1DA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{E45CBD91-B0AD-4D14-BFB4-3F843881D46B}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -660,25 +771,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74491469-0BF1-421A-9748-8AC8795B713A}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{EC7DD9B4-DD25-4431-84C2-EED04403C5CD}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -690,25 +806,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2269D38D-E085-4B69-947B-2B5C26ECC6B1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{61058737-C6BD-45BD-B584-1EDFC740965F}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -720,25 +841,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D87ED03-DF74-4BE7-89EE-AA7970A24159}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{372209F2-C57E-4CF2-8BF9-87D4E50F84AB}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -750,25 +876,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D636556-B298-41D2-9888-FFAD4E5CD8D8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{4FB54264-903A-4DA1-A961-164701BCAB9B}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -780,25 +911,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFA0160C-CDD1-42A6-A8E6-4F746C72BB6F}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{FBF52C24-AF27-4FB0-AE55-AC47D569D2FD}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -810,25 +946,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06BB29E1-5C7D-4B70-A609-BE525B5ECE15}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0C5D7828-6FFC-474A-ABAE-05D07C996862}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -840,25 +981,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18A902B6-BB91-4FD5-B709-5393E650B675}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{9ADBC69F-ED5A-465F-8548-C4E012A6B8E8}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -870,25 +1016,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="13"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{918CD4E5-FC8A-4F6C-949B-7E78149136A8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D1C8F453-1C2B-4E65-A2AF-9D1ED4B90101}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -900,25 +1051,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="14"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9DC051D2-32A5-4507-91B7-8382FAD12220}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{527AD064-2AA9-4771-B68D-5C6B1BD7F509}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -930,25 +1086,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="15"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4687C1F2-E486-4ECC-9CD6-60FBA170C164}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{D8222DEB-126D-4B64-82A7-2682FC3EC999}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -960,25 +1121,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="16"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6AF0FE44-D572-4F76-A1E5-949E322167ED}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{C2B0FBDA-48C8-412D-BB0C-FFBBEE57B463}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -990,25 +1156,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="17"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CAB0B527-C39E-413C-BF8A-CCDAFF3F4998}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0DC220C6-F312-467A-BF51-F39CFD53095F}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1020,25 +1191,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="18"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC2FB84F-FF96-48BF-9CFF-40EB5CE932A4}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{B3CCBB07-5C8E-47AA-B2E8-B1B327C30E26}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1050,25 +1226,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="19"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{781870A7-508E-430E-A5B8-43EDF3C1989D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{A8060E87-FC74-4781-AFB2-760D36CA9F5C}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1080,25 +1261,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="20"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{65520891-405F-4A24-B982-41681C1874F9}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{F533DF2C-76CD-48C3-AB7E-36F3A4550DA4}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1110,25 +1296,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="21"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7826E9D-B5EE-46A2-8C10-E6E84AB5702E}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{5F37F90E-CA5B-403F-B3B8-1A384C1313CA}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1140,25 +1331,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="22"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B288BC7E-98BD-4677-8AE9-89759D8172B4}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0BF8FDF6-57BF-440D-9F5B-99B744DBB4B4}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1170,25 +1366,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="23"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C85AD00-17ED-4EDD-AC99-DE4BEF8D007F}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{68BC005D-7326-4A50-9A13-CA41BF2557B3}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1200,25 +1401,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000017-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="24"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C482FBB-F854-4EDB-9A1B-0F358E0B6872}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{23FBF1A4-9DA1-4CA2-8D85-B859242A36FE}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1230,25 +1436,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000018-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="25"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A93D59F8-900F-4E24-82B4-0E677917A5FA}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{EC1051E2-118B-4B91-8080-4BDA937B44D3}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1260,25 +1471,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000019-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="26"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5A2ACB4-4C92-45EE-833D-D28192A2C1B1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{15480138-560D-4B1D-BF20-7B89226CDAEB}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1290,25 +1506,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001A-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="27"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F924EB0-14F3-41D7-AAAB-83BBE4E6A71D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{264F2A71-CBC8-424B-974A-9D878BCCC6AB}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1320,25 +1541,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001B-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="28"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BBF4A9F6-8BED-4FD2-988D-51C1D20B376D}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{7B2BC180-9968-4446-A97F-5B8D8DA6B614}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1350,25 +1576,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001C-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="29"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6B1BCD0B-3CFE-4940-82D4-A260DDC002E8}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{5626DAF1-1918-482F-873B-809D874C33EA}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1380,25 +1611,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001D-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="30"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87E61112-C826-400E-AC05-040C9005D93C}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{2FD01DB1-0D9B-4B48-863C-1114EEE2224F}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1410,25 +1646,30 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001E-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="31"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5822CF3-9D55-4747-9033-55EC908E3403}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{02F4E841-B549-4D4D-A775-AA78F064BC42}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-US"/>
+                    <a:endParaRPr lang="en-GB"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1440,9 +1681,13 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001F-C3F6-40AB-AA1E-821A545ACD72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1482,8 +1727,9 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1714,10 +1960,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A9B9-4699-85A7-BBCAE1008CF9}"/>
-            </c:ext>
+          <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
                 <c15:f>Data!$B$2:$B$33</c15:f>
@@ -1822,6 +2065,9 @@
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A9B9-4699-85A7-BBCAE1008CF9}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
@@ -2073,7 +2319,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-A9B9-4699-85A7-BBCAE1008CF9}"/>
             </c:ext>
@@ -2224,6 +2470,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2256,7 +2503,7 @@
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
@@ -2852,7 +3099,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2863,13 +3110,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670192" cy="6293013"/>
+    <xdr:ext cx="8663609" cy="6286500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1B75B44A-C79E-43F4-8C15-9CD5F5169534}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B75B44A-C79E-43F4-8C15-9CD5F5169534}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3189,7 +3436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -3198,20 +3445,21 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.3046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.53515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="100.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="81.07421875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="111.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.15234375" style="5"/>
-    <col min="9" max="16384" width="9.15234375" style="1"/>
+    <col min="1" max="1" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="107.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="81.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="111.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="5"/>
+    <col min="9" max="9" width="34.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3233,9 +3481,15 @@
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" s="1">
+      <c r="H1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>14</v>
       </c>
       <c r="B2" s="1">
@@ -3257,12 +3511,16 @@
         <v>68</v>
       </c>
       <c r="H2" s="5" t="str">
-        <f>"curl -O "&amp;G2</f>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_14.html</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="1">
+        <f t="shared" ref="H2:H34" si="0">"curl -O "&amp;F2</f>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_14.zip</v>
+      </c>
+      <c r="I2" s="8" t="str">
+        <f t="shared" ref="I2:I33" si="1">"onix3.0_"&amp;YEAR(C2)&amp;"-"&amp;TEXT(MONTH(C2),"00")&amp;"-"&amp;TEXT(DAY(C2), "00")&amp;"_rev07_codelist"&amp;A2</f>
+        <v>onix3.0_2011-05-31_rev07_codelist14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>15</v>
       </c>
       <c r="B3" s="1">
@@ -3284,12 +3542,16 @@
         <v>69</v>
       </c>
       <c r="H3" s="5" t="str">
-        <f t="shared" ref="H3:H34" si="0">"curl -O "&amp;G3</f>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_15.html</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A4" s="1">
+        <f t="shared" si="0"/>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_15.zip</v>
+      </c>
+      <c r="I3" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2011-07-15_rev07_codelist15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>16</v>
       </c>
       <c r="B4" s="1">
@@ -3312,11 +3574,15 @@
       </c>
       <c r="H4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_16.html</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_16.zip</v>
+      </c>
+      <c r="I4" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2012-01-27_rev07_codelist16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>17</v>
       </c>
       <c r="B5" s="1">
@@ -3339,11 +3605,15 @@
       </c>
       <c r="H5" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_17.html</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A6" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_17.zip</v>
+      </c>
+      <c r="I5" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2012-04-20_rev07_codelist17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>18</v>
       </c>
       <c r="B6" s="1">
@@ -3366,11 +3636,15 @@
       </c>
       <c r="H6" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_18.html</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_18.zip</v>
+      </c>
+      <c r="I6" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2012-04-20_rev07_codelist18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>19</v>
       </c>
       <c r="B7" s="1">
@@ -3393,11 +3667,15 @@
       </c>
       <c r="H7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_19.html</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A8" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_19.zip</v>
+      </c>
+      <c r="I7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2012-10-19_rev07_codelist19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>20</v>
       </c>
       <c r="B8" s="1">
@@ -3420,11 +3698,15 @@
       </c>
       <c r="H8" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_20.html</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_20.zip</v>
+      </c>
+      <c r="I8" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2013-01-25_rev07_codelist20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>21</v>
       </c>
       <c r="B9" s="1">
@@ -3447,11 +3729,15 @@
       </c>
       <c r="H9" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_21.html</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_21.zip</v>
+      </c>
+      <c r="I9" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2013-04-24_rev07_codelist21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>22</v>
       </c>
       <c r="B10" s="1">
@@ -3474,11 +3760,15 @@
       </c>
       <c r="H10" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_22.html</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A11" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_22.zip</v>
+      </c>
+      <c r="I10" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2013-04-24_rev07_codelist22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>23</v>
       </c>
       <c r="B11" s="1">
@@ -3501,11 +3791,15 @@
       </c>
       <c r="H11" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_23.html</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A12" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_23.zip</v>
+      </c>
+      <c r="I11" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2013-04-24_rev07_codelist23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>24</v>
       </c>
       <c r="B12" s="1">
@@ -3528,11 +3822,15 @@
       </c>
       <c r="H12" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_24.html</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A13" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_24.zip</v>
+      </c>
+      <c r="I12" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2014-01-24_rev07_codelist24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>25</v>
       </c>
       <c r="B13" s="1">
@@ -3555,11 +3853,15 @@
       </c>
       <c r="H13" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_25.html</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A14" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_25.zip</v>
+      </c>
+      <c r="I13" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2014-01-24_rev07_codelist25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>26</v>
       </c>
       <c r="B14" s="1">
@@ -3582,11 +3884,15 @@
       </c>
       <c r="H14" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_26.html</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A15" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_26.zip</v>
+      </c>
+      <c r="I14" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2014-06-29_rev07_codelist26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>27</v>
       </c>
       <c r="B15" s="1">
@@ -3609,11 +3915,15 @@
       </c>
       <c r="H15" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_27.html</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A16" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_27.zip</v>
+      </c>
+      <c r="I15" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2014-06-29_rev07_codelist27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>28</v>
       </c>
       <c r="B16" s="1">
@@ -3636,11 +3946,15 @@
       </c>
       <c r="H16" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_28.html</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A17" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_28.zip</v>
+      </c>
+      <c r="I16" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2014-11-23_rev07_codelist28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>29</v>
       </c>
       <c r="B17" s="1">
@@ -3663,11 +3977,15 @@
       </c>
       <c r="H17" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_29.html</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A18" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_29.zip</v>
+      </c>
+      <c r="I17" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2014-11-23_rev07_codelist29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>30</v>
       </c>
       <c r="B18" s="1">
@@ -3690,11 +4008,15 @@
       </c>
       <c r="H18" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_30.html</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_30.zip</v>
+      </c>
+      <c r="I18" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2015-07-29_rev07_codelist30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>31</v>
       </c>
       <c r="B19" s="1">
@@ -3717,11 +4039,15 @@
       </c>
       <c r="H19" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_31.html</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A20" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_31.zip</v>
+      </c>
+      <c r="I19" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2015-07-29_rev07_codelist31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>32</v>
       </c>
       <c r="B20" s="1">
@@ -3744,11 +4070,15 @@
       </c>
       <c r="H20" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_32.html</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_32.zip</v>
+      </c>
+      <c r="I20" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2016-01-24_rev07_codelist32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>33</v>
       </c>
       <c r="B21" s="1">
@@ -3771,11 +4101,15 @@
       </c>
       <c r="H21" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_33.html</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A22" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_33.zip</v>
+      </c>
+      <c r="I21" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2016-04-25_rev07_codelist33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>34</v>
       </c>
       <c r="B22" s="1">
@@ -3798,11 +4132,15 @@
       </c>
       <c r="H22" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_34.html</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A23" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_34.zip</v>
+      </c>
+      <c r="I22" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2016-04-25_rev07_codelist34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>35</v>
       </c>
       <c r="B23" s="1">
@@ -3825,11 +4163,15 @@
       </c>
       <c r="H23" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_35.html</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A24" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_35.zip</v>
+      </c>
+      <c r="I23" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2016-04-25_rev07_codelist35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>36</v>
       </c>
       <c r="B24" s="1">
@@ -3852,11 +4194,15 @@
       </c>
       <c r="H24" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_36.html</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A25" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_36.zip</v>
+      </c>
+      <c r="I24" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2016-04-25_rev07_codelist36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>37</v>
       </c>
       <c r="B25" s="1">
@@ -3879,11 +4225,15 @@
       </c>
       <c r="H25" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_37.html</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_37.zip</v>
+      </c>
+      <c r="I25" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2016-04-25_rev07_codelist37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>38</v>
       </c>
       <c r="B26" s="1">
@@ -3906,11 +4256,15 @@
       </c>
       <c r="H26" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_38.html</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A27" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_38.zip</v>
+      </c>
+      <c r="I26" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2016-04-25_rev07_codelist38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>39</v>
       </c>
       <c r="B27" s="1">
@@ -3933,11 +4287,15 @@
       </c>
       <c r="H27" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_39.html</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A28" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_39.zip</v>
+      </c>
+      <c r="I27" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2017-10-26_rev07_codelist39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>40</v>
       </c>
       <c r="B28" s="1">
@@ -3960,11 +4318,15 @@
       </c>
       <c r="H28" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_40.html</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A29" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_40.zip</v>
+      </c>
+      <c r="I28" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2017-10-26_rev07_codelist40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>41</v>
       </c>
       <c r="B29" s="1">
@@ -3987,11 +4349,15 @@
       </c>
       <c r="H29" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_41.html</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A30" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_41.zip</v>
+      </c>
+      <c r="I29" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2017-10-26_rev07_codelist41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>42</v>
       </c>
       <c r="B30" s="1">
@@ -4014,11 +4380,15 @@
       </c>
       <c r="H30" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_42.html</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A31" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_42.zip</v>
+      </c>
+      <c r="I30" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2017-10-26_rev07_codelist42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>43</v>
       </c>
       <c r="B31" s="1">
@@ -4041,11 +4411,15 @@
       </c>
       <c r="H31" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_43.html</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A32" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_43.zip</v>
+      </c>
+      <c r="I31" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2018-10-26_rev07_codelist43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>44</v>
       </c>
       <c r="B32" s="1">
@@ -4068,11 +4442,15 @@
       </c>
       <c r="H32" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_44.html</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A33" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_44.zip</v>
+      </c>
+      <c r="I32" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2018-10-26_rev07_codelist44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>45</v>
       </c>
       <c r="B33" s="1">
@@ -4095,11 +4473,15 @@
       </c>
       <c r="H33" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_45.html</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A34" s="1">
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_45.zip</v>
+      </c>
+      <c r="I33" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>onix3.0_2019-04-26_rev07_codelist45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>49</v>
       </c>
       <c r="B34" s="1">
@@ -4111,7 +4493,7 @@
       <c r="D34" s="3">
         <v>43907</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>103</v>
       </c>
       <c r="F34" s="1" t="s">
@@ -4122,11 +4504,736 @@
       </c>
       <c r="H34" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>curl -O https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_49.html</v>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_49.zip</v>
+      </c>
+      <c r="I34" s="8" t="str">
+        <f>"onix3.0_"&amp;YEAR(C34)&amp;"-"&amp;TEXT(MONTH(C34),"00")&amp;"-"&amp;TEXT(DAY(C34), "00")&amp;"_rev07_codelist"&amp;A34</f>
+        <v>onix3.0_2019-10-31_rev07_codelist49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>50</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="C35" s="6">
+        <v>43969</v>
+      </c>
+      <c r="D35" s="6">
+        <v>44021</v>
+      </c>
+      <c r="E35" t="s">
+        <v>119</v>
+      </c>
+      <c r="F35" s="1" t="str">
+        <f>"https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_"&amp;A35&amp;".zip"</f>
+        <v>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_50.zip</v>
+      </c>
+      <c r="G35" s="1" t="str">
+        <f>"https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_"&amp;A35&amp;".html"</f>
+        <v>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_50.html</v>
+      </c>
+      <c r="H35" s="5" t="str">
+        <f>"curl -O "&amp;F35</f>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_50.zip</v>
+      </c>
+      <c r="I35" s="8" t="str">
+        <f>"onix3.0_"&amp;YEAR(C35)&amp;"-"&amp;TEXT(MONTH(C35),"00")&amp;"-"&amp;TEXT(DAY(C35), "00")&amp;"_rev"&amp;TEXT(B35, "00")&amp;"_codelist"&amp;A35</f>
+        <v>onix3.0_2020-05-18_rev07_codelist50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>51</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" s="6">
+        <v>43969</v>
+      </c>
+      <c r="D36" s="6">
+        <v>44124</v>
+      </c>
+      <c r="E36" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="1" t="str">
+        <f t="shared" ref="F36:F43" si="2">"https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_"&amp;A36&amp;".zip"</f>
+        <v>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_51.zip</v>
+      </c>
+      <c r="G36" s="1" t="str">
+        <f t="shared" ref="G36:G43" si="3">"https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_"&amp;A36&amp;".html"</f>
+        <v>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_51.html</v>
+      </c>
+      <c r="H36" s="5" t="str">
+        <f t="shared" ref="H36:H43" si="4">"curl -O "&amp;F36</f>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_51.zip</v>
+      </c>
+      <c r="I36" s="8" t="str">
+        <f t="shared" ref="I36:I43" si="5">"onix3.0_"&amp;YEAR(C36)&amp;"-"&amp;TEXT(MONTH(C36),"00")&amp;"-"&amp;TEXT(DAY(C36), "00")&amp;"_rev"&amp;TEXT(B36, "00")&amp;"_codelist"&amp;A36</f>
+        <v>onix3.0_2020-05-18_rev07_codelist51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>52</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37" s="6">
+        <v>43969</v>
+      </c>
+      <c r="D37" s="6">
+        <v>44221</v>
+      </c>
+      <c r="E37" t="s">
+        <v>123</v>
+      </c>
+      <c r="F37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_52.zip</v>
+      </c>
+      <c r="G37" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_52.html</v>
+      </c>
+      <c r="H37" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_52.zip</v>
+      </c>
+      <c r="I37" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>onix3.0_2020-05-18_rev07_codelist52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>53</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38" s="6">
+        <v>44315</v>
+      </c>
+      <c r="D38" s="6">
+        <v>44376</v>
+      </c>
+      <c r="E38" t="s">
+        <v>124</v>
+      </c>
+      <c r="F38" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_53.zip</v>
+      </c>
+      <c r="G38" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_53.html</v>
+      </c>
+      <c r="H38" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_53.zip</v>
+      </c>
+      <c r="I38" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>onix3.0_2021-04-29_rev08_codelist53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>54</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39" s="6">
+        <v>44315</v>
+      </c>
+      <c r="D39" s="6">
+        <v>44416</v>
+      </c>
+      <c r="E39" t="s">
+        <v>125</v>
+      </c>
+      <c r="F39" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_54.zip</v>
+      </c>
+      <c r="G39" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_54.html</v>
+      </c>
+      <c r="H39" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_54.zip</v>
+      </c>
+      <c r="I39" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>onix3.0_2021-04-29_rev08_codelist54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>55</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40" s="6">
+        <v>44315</v>
+      </c>
+      <c r="D40" s="6">
+        <v>44497</v>
+      </c>
+      <c r="E40" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_55.zip</v>
+      </c>
+      <c r="G40" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_55.html</v>
+      </c>
+      <c r="H40" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_55.zip</v>
+      </c>
+      <c r="I40" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>onix3.0_2021-04-29_rev08_codelist55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>56</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41" s="6">
+        <v>44315</v>
+      </c>
+      <c r="D41" s="6">
+        <v>44582</v>
+      </c>
+      <c r="E41" t="s">
+        <v>120</v>
+      </c>
+      <c r="F41" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_56.zip</v>
+      </c>
+      <c r="G41" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_56.html</v>
+      </c>
+      <c r="H41" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_56.zip</v>
+      </c>
+      <c r="I41" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>onix3.0_2021-04-29_rev08_codelist56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>57</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42" s="6">
+        <v>44315</v>
+      </c>
+      <c r="D42" s="6">
+        <v>44663</v>
+      </c>
+      <c r="E42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_57.zip</v>
+      </c>
+      <c r="G42" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_57.html</v>
+      </c>
+      <c r="H42" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_57.zip</v>
+      </c>
+      <c r="I42" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>onix3.0_2021-04-29_rev08_codelist57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>58</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43" s="6">
+        <v>44315</v>
+      </c>
+      <c r="D43" s="6">
+        <v>44760</v>
+      </c>
+      <c r="E43" t="s">
+        <v>127</v>
+      </c>
+      <c r="F43" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_58.zip</v>
+      </c>
+      <c r="G43" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>https://www.editeur.org/files/ONIX%20for%20books%20-%20code%20lists/ONIX_BookProduct_Codelists_Issue_58.html</v>
+      </c>
+      <c r="H43" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>curl -O https://www.editeur.org/files/ONIX%203/ONIX_BookProduct_XSD_schema+codes_Issue_58.zip</v>
+      </c>
+      <c r="I43" s="8" t="str">
+        <f t="shared" si="5"/>
+        <v>onix3.0_2021-04-29_rev08_codelist58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32:G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="str">
+        <f>MID(A2,33,10)</f>
+        <v>2020-05-18</v>
+      </c>
+      <c r="E2" t="str">
+        <f>MID(A21,36,10)</f>
+        <v>2020-07-09</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3">
+        <f>B1+1</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B18" si="0">B2+1</f>
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="str">
+        <f>MID(A4,33,10)</f>
+        <v>2020-05-18</v>
+      </c>
+      <c r="E4" t="str">
+        <f>MID(A22,36,10)</f>
+        <v>2020-10-20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="str">
+        <f>MID(A6,33,10)</f>
+        <v>2020-05-18</v>
+      </c>
+      <c r="E6" t="str">
+        <f>MID(A23,36,10)</f>
+        <v>2021-01-25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="str">
+        <f>MID(A8,33,10)</f>
+        <v>2021-04-29</v>
+      </c>
+      <c r="E8" t="str">
+        <f>MID(A24,36,10)</f>
+        <v>2021-06-29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="str">
+        <f>MID(A10,33,10)</f>
+        <v>2021-04-29</v>
+      </c>
+      <c r="E10" t="str">
+        <f>MID(A25,36,10)</f>
+        <v>2021-08-08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="str">
+        <f>MID(A12,33,10)</f>
+        <v>2021-04-29</v>
+      </c>
+      <c r="E12" t="str">
+        <f>MID(A26,36,10)</f>
+        <v>2021-10-28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="str">
+        <f>MID(A14,33,10)</f>
+        <v>2021-04-29</v>
+      </c>
+      <c r="E14" t="str">
+        <f>MID(A27,36,10)</f>
+        <v>2022-01-21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="str">
+        <f>MID(A16,33,10)</f>
+        <v>2021-04-29</v>
+      </c>
+      <c r="E16" t="str">
+        <f>MID(A28,36,10)</f>
+        <v>2022-04-12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="str">
+        <f>MID(A18,33,10)</f>
+        <v>2021-04-29</v>
+      </c>
+      <c r="E18" t="str">
+        <f>MID(A29,36,10)</f>
+        <v>2022-07-18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32" s="6">
+        <v>43969</v>
+      </c>
+      <c r="G32" s="6">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33" s="6">
+        <v>43969</v>
+      </c>
+      <c r="G33" s="6">
+        <v>44124</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34" s="6">
+        <v>43969</v>
+      </c>
+      <c r="G34" s="6">
+        <v>44221</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35" s="6">
+        <v>44315</v>
+      </c>
+      <c r="G35" s="6">
+        <v>44376</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36" s="6">
+        <v>44315</v>
+      </c>
+      <c r="G36" s="6">
+        <v>44416</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>8</v>
+      </c>
+      <c r="F37" s="6">
+        <v>44315</v>
+      </c>
+      <c r="G37" s="6">
+        <v>44497</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38" s="6">
+        <v>44315</v>
+      </c>
+      <c r="G38" s="6">
+        <v>44582</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39" s="6">
+        <v>44315</v>
+      </c>
+      <c r="G39" s="6">
+        <v>44663</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40" s="6">
+        <v>44315</v>
+      </c>
+      <c r="G40" s="6">
+        <v>44760</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>